<commit_message>
build based on e180346
</commit_message>
<xml_diff>
--- a/dev/results/output_file_NC.xlsx
+++ b/dev/results/output_file_NC.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
   <si>
     <t>comp_time</t>
   </si>
@@ -51,6 +51,9 @@
     <t>x_us_PV</t>
   </si>
   <si>
+    <t>x_us_generator</t>
+  </si>
+  <si>
     <t>x_us_batt</t>
   </si>
   <si>
@@ -81,6 +84,9 @@
     <t>yearly_rev</t>
   </si>
   <si>
+    <t>C_gen_tot_us</t>
+  </si>
+  <si>
     <t>SDCF C_OEM_tot_us</t>
   </si>
   <si>
@@ -102,6 +108,9 @@
     <t>CAPEX_us_PV</t>
   </si>
   <si>
+    <t>CAPEX_us_generator</t>
+  </si>
+  <si>
     <t>CAPEX_us_batt</t>
   </si>
   <si>
@@ -115,6 +124,9 @@
   </si>
   <si>
     <t>C_OEM_us_PV</t>
+  </si>
+  <si>
+    <t>C_OEM_us_generator</t>
   </si>
   <si>
     <t>C_OEM_us_batt</t>
@@ -527,7 +539,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>1.2853541374206543</v>
+        <v>2.055131196975708</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -540,13 +552,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -571,10 +583,13 @@
       <c r="H1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>55.29324587</v>
@@ -586,13 +601,16 @@
       <c r="E2">
         <v>50.0</v>
       </c>
-      <c r="F2"/>
+      <c r="F2">
+        <v>0.0</v>
+      </c>
       <c r="G2"/>
       <c r="H2"/>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2"/>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>27.00540954</v>
@@ -604,17 +622,18 @@
       <c r="E3">
         <v>25.489185845443384</v>
       </c>
-      <c r="F3">
-        <v>1.973245920368238</v>
-      </c>
+      <c r="F3"/>
       <c r="G3">
         <v>1.973245920368238</v>
       </c>
-      <c r="H3"/>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="H3">
+        <v>1.973245920368238</v>
+      </c>
+      <c r="I3"/>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>45.40292054</v>
@@ -624,16 +643,17 @@
       </c>
       <c r="D4"/>
       <c r="E4">
-        <v>44.04652629600474</v>
-      </c>
-      <c r="F4">
-        <v>3.7213684553918602</v>
-      </c>
+        <v>44.04652629600476</v>
+      </c>
+      <c r="F4"/>
       <c r="G4">
-        <v>3.7213684553918602</v>
+        <v>3.721368455391854</v>
       </c>
       <c r="H4">
-        <v>34.906983718279804</v>
+        <v>3.721368455391854</v>
+      </c>
+      <c r="I4">
+        <v>34.906983718279776</v>
       </c>
     </row>
   </sheetData>
@@ -643,74 +663,83 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19">
+        <v>32</v>
+      </c>
+      <c r="T1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>-563669.0832118867</v>
@@ -722,139 +751,158 @@
         <v>-31580.287385073458</v>
       </c>
       <c r="E2">
+        <v>-8.573955168024072e-14</v>
+      </c>
+      <c r="F2">
         <v>22316.212290683256</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.0</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>9412.487821167684</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>18246.63937566448</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>-447518.7193667072</v>
       </c>
-      <c r="J2"/>
-      <c r="K2">
+      <c r="K2"/>
+      <c r="L2">
         <v>85000.0</v>
       </c>
-      <c r="L2"/>
-      <c r="M2"/>
+      <c r="M2">
+        <v>0.0</v>
+      </c>
       <c r="N2"/>
       <c r="O2"/>
-      <c r="P2">
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2">
         <v>1500.0</v>
       </c>
-      <c r="Q2"/>
-      <c r="R2"/>
-      <c r="S2"/>
-    </row>
-    <row r="3" spans="1:19">
+      <c r="S2">
+        <v>0.0</v>
+      </c>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+    </row>
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3">
-        <v>-223241.12057109867</v>
+        <v>-223241.12057109879</v>
       </c>
       <c r="C3">
         <v>36868.807735841685</v>
       </c>
       <c r="D3">
-        <v>-12164.328747674772</v>
+        <v>-12164.328747674768</v>
       </c>
       <c r="E3">
+        <v>0.0</v>
+      </c>
+      <c r="F3">
         <v>11581.94006488829</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>800.2766440442327</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>4242.911954548019</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>8840.453007913167</v>
       </c>
-      <c r="I3">
-        <v>-169392.5550729593</v>
-      </c>
-      <c r="J3"/>
-      <c r="K3">
+      <c r="J3">
+        <v>-169392.55507295928</v>
+      </c>
+      <c r="K3"/>
+      <c r="L3">
         <v>35684.86018362074</v>
       </c>
-      <c r="L3">
+      <c r="M3"/>
+      <c r="N3">
         <v>789.2983681472952</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>394.6491840736476</v>
       </c>
-      <c r="N3"/>
-      <c r="O3"/>
-      <c r="P3">
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3">
         <v>764.6755753633015</v>
       </c>
-      <c r="Q3">
+      <c r="S3"/>
+      <c r="T3">
         <v>9.86622960184119</v>
       </c>
-      <c r="R3">
+      <c r="U3">
         <v>3.946491840736476</v>
       </c>
-      <c r="S3"/>
-    </row>
-    <row r="4" spans="1:19">
+      <c r="V3"/>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>-435831.69036038255</v>
       </c>
       <c r="C4">
-        <v>177428.2143016821</v>
+        <v>177428.21430168205</v>
       </c>
       <c r="D4">
-        <v>-17171.222950664825</v>
+        <v>-17171.222950664833</v>
       </c>
       <c r="E4">
-        <v>35626.4177709583</v>
+        <v>0.0</v>
       </c>
       <c r="F4">
-        <v>1509.251446052555</v>
+        <v>35626.41777095829</v>
       </c>
       <c r="G4">
+        <v>1509.2514460525526</v>
+      </c>
+      <c r="H4">
         <v>8353.446369498317</v>
       </c>
-      <c r="H4">
-        <v>9783.233210352735</v>
-      </c>
       <c r="I4">
-        <v>-219838.02000083425</v>
-      </c>
-      <c r="J4"/>
-      <c r="K4">
-        <v>70474.44207360758</v>
-      </c>
+        <v>9783.233210352739</v>
+      </c>
+      <c r="J4">
+        <v>-219838.02000083437</v>
+      </c>
+      <c r="K4"/>
       <c r="L4">
-        <v>1488.547382156744</v>
-      </c>
-      <c r="M4">
-        <v>744.273691078372</v>
-      </c>
+        <v>70474.44207360761</v>
+      </c>
+      <c r="M4"/>
       <c r="N4">
-        <v>104720.95115483941</v>
-      </c>
-      <c r="O4"/>
+        <v>1488.5473821567416</v>
+      </c>
+      <c r="O4">
+        <v>744.2736910783708</v>
+      </c>
       <c r="P4">
-        <v>1321.3957888801424</v>
-      </c>
-      <c r="Q4">
-        <v>18.606842276959302</v>
-      </c>
+        <v>104720.95115483932</v>
+      </c>
+      <c r="Q4"/>
       <c r="R4">
-        <v>7.4427369107837205</v>
-      </c>
-      <c r="S4">
-        <v>1047.2095115483942</v>
+        <v>1321.3957888801426</v>
+      </c>
+      <c r="S4"/>
+      <c r="T4">
+        <v>18.60684227695927</v>
+      </c>
+      <c r="U4">
+        <v>7.442736910783708</v>
+      </c>
+      <c r="V4">
+        <v>1047.2095115483933</v>
       </c>
     </row>
   </sheetData>
@@ -872,48 +920,48 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="J1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="K1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="L1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="M1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>50.3983545</v>
@@ -955,7 +1003,7 @@
         <v>23.93422539963176</v>
       </c>
       <c r="O2">
-        <v>32.86113926823138</v>
+        <v>32.8611392682314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>